<commit_message>
Commit on 14th jan 2016
</commit_message>
<xml_diff>
--- a/Excels/Data_QA_Tests.xlsx
+++ b/Excels/Data_QA_Tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sahi_pro\userdata\12twenty\excels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="11760" tabRatio="661" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="11760" tabRatio="661"/>
   </bookViews>
   <sheets>
     <sheet name="MBA Standard Reports" sheetId="1" r:id="rId1"/>
@@ -1602,8 +1607,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1890,6 +1895,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1936,7 +1949,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1968,9 +1981,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2002,6 +2016,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2177,14 +2192,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -2197,7 +2212,7 @@
     <col min="15" max="15" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="31.5" customHeight="1">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>41</v>
       </c>
@@ -2244,7 +2259,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>525</v>
       </c>
@@ -2338,7 +2353,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>525</v>
       </c>
@@ -2385,7 +2400,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>525</v>
       </c>
@@ -2432,7 +2447,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>525</v>
       </c>
@@ -2479,7 +2494,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>525</v>
       </c>
@@ -2526,7 +2541,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>525</v>
       </c>
@@ -2573,7 +2588,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>525</v>
       </c>
@@ -2620,7 +2635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>525</v>
       </c>
@@ -2667,7 +2682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>525</v>
       </c>
@@ -2714,7 +2729,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>525</v>
       </c>
@@ -2761,7 +2776,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>525</v>
       </c>
@@ -2808,7 +2823,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>525</v>
       </c>
@@ -2855,7 +2870,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>525</v>
       </c>
@@ -2902,7 +2917,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>525</v>
       </c>
@@ -2949,7 +2964,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>525</v>
       </c>
@@ -2996,7 +3011,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>525</v>
       </c>
@@ -3043,7 +3058,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>525</v>
       </c>
@@ -3090,7 +3105,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>525</v>
       </c>
@@ -3137,7 +3152,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>525</v>
       </c>
@@ -3184,7 +3199,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>525</v>
       </c>
@@ -3231,7 +3246,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>525</v>
       </c>
@@ -3278,7 +3293,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>525</v>
       </c>
@@ -3325,7 +3340,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>525</v>
       </c>
@@ -3372,7 +3387,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>525</v>
       </c>
@@ -3419,7 +3434,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>525</v>
       </c>
@@ -3466,7 +3481,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>525</v>
       </c>
@@ -3513,7 +3528,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>525</v>
       </c>
@@ -3560,7 +3575,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>525</v>
       </c>
@@ -3607,7 +3622,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>525</v>
       </c>
@@ -3654,7 +3669,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>525</v>
       </c>
@@ -3701,7 +3716,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>525</v>
       </c>
@@ -3748,7 +3763,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>525</v>
       </c>
@@ -3795,7 +3810,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>525</v>
       </c>
@@ -3842,7 +3857,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>525</v>
       </c>
@@ -3889,7 +3904,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>525</v>
       </c>
@@ -3936,7 +3951,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>525</v>
       </c>
@@ -3983,7 +3998,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>525</v>
       </c>
@@ -4030,7 +4045,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>525</v>
       </c>
@@ -4077,7 +4092,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>525</v>
       </c>
@@ -4124,7 +4139,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="26.25">
+    <row r="42" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>525</v>
       </c>
@@ -4171,7 +4186,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="26.25">
+    <row r="43" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>525</v>
       </c>
@@ -4218,7 +4233,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="26.25">
+    <row r="44" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>525</v>
       </c>
@@ -4265,7 +4280,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="26.25">
+    <row r="45" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>525</v>
       </c>
@@ -4312,7 +4327,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="26.25">
+    <row r="46" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>525</v>
       </c>
@@ -4359,7 +4374,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="26.25">
+    <row r="47" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>525</v>
       </c>
@@ -4406,7 +4421,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="26.25">
+    <row r="48" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>525</v>
       </c>
@@ -4453,7 +4468,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="26.25">
+    <row r="49" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>525</v>
       </c>
@@ -4500,7 +4515,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="26.25">
+    <row r="50" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>525</v>
       </c>
@@ -4547,7 +4562,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="26.25">
+    <row r="51" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>525</v>
       </c>
@@ -4594,7 +4609,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>525</v>
       </c>
@@ -4641,7 +4656,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>525</v>
       </c>
@@ -4688,7 +4703,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>525</v>
       </c>
@@ -4735,7 +4750,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>525</v>
       </c>
@@ -4782,7 +4797,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>525</v>
       </c>
@@ -4829,7 +4844,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>525</v>
       </c>
@@ -4876,7 +4891,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>525</v>
       </c>
@@ -4923,7 +4938,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>525</v>
       </c>
@@ -4970,7 +4985,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>525</v>
       </c>
@@ -5017,7 +5032,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>525</v>
       </c>
@@ -5057,14 +5072,14 @@
       <c r="M61" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N61" s="21" t="s">
+      <c r="N61" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O61" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="26.25">
+    <row r="62" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>525</v>
       </c>
@@ -5111,7 +5126,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="26.25">
+    <row r="63" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>525</v>
       </c>
@@ -5158,7 +5173,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="26.25">
+    <row r="64" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>525</v>
       </c>
@@ -5205,7 +5220,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="26.25">
+    <row r="65" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>525</v>
       </c>
@@ -5252,7 +5267,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="26.25">
+    <row r="66" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>525</v>
       </c>
@@ -5299,7 +5314,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="26.25">
+    <row r="67" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>525</v>
       </c>
@@ -5346,7 +5361,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="26.25">
+    <row r="68" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>525</v>
       </c>
@@ -5393,7 +5408,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="26.25">
+    <row r="69" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>525</v>
       </c>
@@ -5440,7 +5455,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="26.25">
+    <row r="70" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>525</v>
       </c>
@@ -5487,7 +5502,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="26.25">
+    <row r="71" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>525</v>
       </c>
@@ -5534,7 +5549,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>525</v>
       </c>
@@ -5581,7 +5596,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>525</v>
       </c>
@@ -5628,7 +5643,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>525</v>
       </c>
@@ -5675,7 +5690,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>525</v>
       </c>
@@ -5722,7 +5737,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>525</v>
       </c>
@@ -5769,7 +5784,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>525</v>
       </c>
@@ -5816,7 +5831,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>525</v>
       </c>
@@ -5863,7 +5878,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>525</v>
       </c>
@@ -5910,7 +5925,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>525</v>
       </c>
@@ -5957,7 +5972,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>525</v>
       </c>
@@ -6004,7 +6019,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>525</v>
       </c>
@@ -6051,7 +6066,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>525</v>
       </c>
@@ -6098,7 +6113,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>525</v>
       </c>
@@ -6145,7 +6160,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>525</v>
       </c>
@@ -6192,7 +6207,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>525</v>
       </c>
@@ -6239,7 +6254,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>525</v>
       </c>
@@ -6286,7 +6301,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>525</v>
       </c>
@@ -6333,7 +6348,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>525</v>
       </c>
@@ -6380,7 +6395,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>525</v>
       </c>
@@ -6427,7 +6442,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>525</v>
       </c>
@@ -6474,7 +6489,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="26.25">
+    <row r="92" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>525</v>
       </c>
@@ -6521,7 +6536,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="26.25">
+    <row r="93" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>525</v>
       </c>
@@ -6568,7 +6583,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="26.25">
+    <row r="94" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>525</v>
       </c>
@@ -6615,7 +6630,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="26.25">
+    <row r="95" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>525</v>
       </c>
@@ -6662,7 +6677,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="26.25">
+    <row r="96" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>525</v>
       </c>
@@ -6709,7 +6724,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="26.25">
+    <row r="97" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>525</v>
       </c>
@@ -6756,7 +6771,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="26.25">
+    <row r="98" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>525</v>
       </c>
@@ -6803,7 +6818,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="26.25">
+    <row r="99" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>525</v>
       </c>
@@ -6850,7 +6865,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="26.25">
+    <row r="100" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>525</v>
       </c>
@@ -6897,7 +6912,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="26.25">
+    <row r="101" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>525</v>
       </c>
@@ -6944,7 +6959,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="26.25">
+    <row r="102" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>525</v>
       </c>
@@ -6991,7 +7006,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="26.25">
+    <row r="103" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>525</v>
       </c>
@@ -7038,7 +7053,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="26.25">
+    <row r="104" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>525</v>
       </c>
@@ -7085,7 +7100,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="26.25">
+    <row r="105" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>525</v>
       </c>
@@ -7132,7 +7147,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="26.25">
+    <row r="106" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>525</v>
       </c>
@@ -7179,7 +7194,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="26.25">
+    <row r="107" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>525</v>
       </c>
@@ -7226,7 +7241,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="26.25">
+    <row r="108" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>525</v>
       </c>
@@ -7273,7 +7288,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="26.25">
+    <row r="109" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>525</v>
       </c>
@@ -7320,7 +7335,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="26.25">
+    <row r="110" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>525</v>
       </c>
@@ -7367,7 +7382,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="26.25">
+    <row r="111" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>525</v>
       </c>
@@ -7414,7 +7429,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="26.25">
+    <row r="112" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>525</v>
       </c>
@@ -7461,7 +7476,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="26.25">
+    <row r="113" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>525</v>
       </c>
@@ -7508,7 +7523,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="26.25">
+    <row r="114" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>525</v>
       </c>
@@ -7555,7 +7570,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="26.25">
+    <row r="115" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>525</v>
       </c>
@@ -7602,7 +7617,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="26.25">
+    <row r="116" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>525</v>
       </c>
@@ -7649,7 +7664,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="26.25">
+    <row r="117" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>525</v>
       </c>
@@ -7696,7 +7711,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="26.25">
+    <row r="118" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>525</v>
       </c>
@@ -7743,7 +7758,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="26.25">
+    <row r="119" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>525</v>
       </c>
@@ -7790,7 +7805,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="26.25">
+    <row r="120" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>525</v>
       </c>
@@ -7837,7 +7852,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="26.25">
+    <row r="121" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>525</v>
       </c>
@@ -7891,14 +7906,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -7913,7 +7928,7 @@
     <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="31.5" customHeight="1">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>41</v>
       </c>
@@ -7961,7 +7976,7 @@
       </c>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>525</v>
       </c>
@@ -8009,7 +8024,7 @@
       </c>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>525</v>
       </c>
@@ -8057,7 +8072,7 @@
       </c>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>525</v>
       </c>
@@ -8105,7 +8120,7 @@
       </c>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>525</v>
       </c>
@@ -8153,7 +8168,7 @@
       </c>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>525</v>
       </c>
@@ -8201,7 +8216,7 @@
       </c>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>525</v>
       </c>
@@ -8249,7 +8264,7 @@
       </c>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>525</v>
       </c>
@@ -8297,7 +8312,7 @@
       </c>
       <c r="P8" s="13"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>525</v>
       </c>
@@ -8345,7 +8360,7 @@
       </c>
       <c r="P9" s="13"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>525</v>
       </c>
@@ -8393,7 +8408,7 @@
       </c>
       <c r="P10" s="13"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>525</v>
       </c>
@@ -8441,7 +8456,7 @@
       </c>
       <c r="P11" s="13"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>525</v>
       </c>
@@ -8489,7 +8504,7 @@
       </c>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>525</v>
       </c>
@@ -8537,7 +8552,7 @@
       </c>
       <c r="P13" s="13"/>
     </row>
-    <row r="14" spans="1:16" ht="26.25">
+    <row r="14" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>525</v>
       </c>
@@ -8585,7 +8600,7 @@
       </c>
       <c r="P14" s="13"/>
     </row>
-    <row r="15" spans="1:16" ht="26.25">
+    <row r="15" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>525</v>
       </c>
@@ -8633,7 +8648,7 @@
       </c>
       <c r="P15" s="13"/>
     </row>
-    <row r="16" spans="1:16" ht="26.25">
+    <row r="16" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>525</v>
       </c>
@@ -8681,7 +8696,7 @@
       </c>
       <c r="P16" s="13"/>
     </row>
-    <row r="17" spans="1:16" ht="26.25">
+    <row r="17" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>525</v>
       </c>
@@ -8729,7 +8744,7 @@
       </c>
       <c r="P17" s="13"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>525</v>
       </c>
@@ -8777,7 +8792,7 @@
       </c>
       <c r="P18" s="13"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>525</v>
       </c>
@@ -8825,7 +8840,7 @@
       </c>
       <c r="P19" s="13"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>525</v>
       </c>
@@ -8873,7 +8888,7 @@
       </c>
       <c r="P20" s="13"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>525</v>
       </c>
@@ -8921,7 +8936,7 @@
       </c>
       <c r="P21" s="13"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
         <v>525</v>
       </c>
@@ -8969,7 +8984,7 @@
       </c>
       <c r="P22" s="13"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="62" t="s">
         <v>525</v>
       </c>
@@ -9017,7 +9032,7 @@
       </c>
       <c r="P23" s="13"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>525</v>
       </c>
@@ -9065,7 +9080,7 @@
       </c>
       <c r="P24" s="13"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>525</v>
       </c>
@@ -9113,7 +9128,7 @@
       </c>
       <c r="P25" s="13"/>
     </row>
-    <row r="26" spans="1:16" ht="26.25">
+    <row r="26" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
         <v>525</v>
       </c>
@@ -9161,7 +9176,7 @@
       </c>
       <c r="P26" s="13"/>
     </row>
-    <row r="27" spans="1:16" ht="26.25">
+    <row r="27" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="62" t="s">
         <v>525</v>
       </c>
@@ -9209,7 +9224,7 @@
       </c>
       <c r="P27" s="13"/>
     </row>
-    <row r="28" spans="1:16" ht="26.25">
+    <row r="28" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
         <v>525</v>
       </c>
@@ -9257,7 +9272,7 @@
       </c>
       <c r="P28" s="13"/>
     </row>
-    <row r="29" spans="1:16" ht="26.25">
+    <row r="29" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="62" t="s">
         <v>525</v>
       </c>
@@ -9305,7 +9320,7 @@
       </c>
       <c r="P29" s="13"/>
     </row>
-    <row r="30" spans="1:16" ht="26.25">
+    <row r="30" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="s">
         <v>525</v>
       </c>
@@ -9353,7 +9368,7 @@
       </c>
       <c r="P30" s="13"/>
     </row>
-    <row r="31" spans="1:16" ht="26.25">
+    <row r="31" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
         <v>525</v>
       </c>
@@ -9401,7 +9416,7 @@
       </c>
       <c r="P31" s="13"/>
     </row>
-    <row r="32" spans="1:16" ht="26.25">
+    <row r="32" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="s">
         <v>525</v>
       </c>
@@ -9449,7 +9464,7 @@
       </c>
       <c r="P32" s="13"/>
     </row>
-    <row r="33" spans="1:16" ht="26.25">
+    <row r="33" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
         <v>525</v>
       </c>
@@ -9497,7 +9512,7 @@
       </c>
       <c r="P33" s="13"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="s">
         <v>525</v>
       </c>
@@ -9545,9 +9560,9 @@
       </c>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>19</v>
@@ -9593,9 +9608,9 @@
       </c>
       <c r="P35" s="13"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>19</v>
@@ -9641,9 +9656,9 @@
       </c>
       <c r="P36" s="13"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>19</v>
@@ -9689,9 +9704,9 @@
       </c>
       <c r="P37" s="13"/>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>19</v>
@@ -9737,7 +9752,7 @@
       </c>
       <c r="P38" s="13"/>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="62" t="s">
         <v>525</v>
       </c>
@@ -9785,7 +9800,7 @@
       </c>
       <c r="P39" s="13"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="62" t="s">
         <v>525</v>
       </c>
@@ -9833,7 +9848,7 @@
       </c>
       <c r="P40" s="13"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="s">
         <v>525</v>
       </c>
@@ -9888,14 +9903,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
@@ -9914,7 +9929,7 @@
     <col min="15" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="37.5" customHeight="1">
+    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>41</v>
       </c>
@@ -9962,7 +9977,7 @@
       </c>
       <c r="P1" s="66"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
         <v>525</v>
       </c>
@@ -10009,7 +10024,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
         <v>525</v>
       </c>
@@ -10056,7 +10071,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
         <v>525</v>
       </c>
@@ -10103,7 +10118,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
         <v>525</v>
       </c>
@@ -10150,7 +10165,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
         <v>525</v>
       </c>
@@ -10197,7 +10212,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
         <v>525</v>
       </c>
@@ -10244,7 +10259,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
         <v>525</v>
       </c>
@@ -10291,7 +10306,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
         <v>525</v>
       </c>
@@ -10338,7 +10353,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>525</v>
       </c>
@@ -10381,7 +10396,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
         <v>525</v>
       </c>
@@ -10424,7 +10439,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
         <v>525</v>
       </c>
@@ -10471,7 +10486,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>525</v>
       </c>
@@ -10518,7 +10533,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
         <v>525</v>
       </c>
@@ -10565,7 +10580,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
         <v>525</v>
       </c>
@@ -10612,7 +10627,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
         <v>525</v>
       </c>
@@ -10659,7 +10674,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="s">
         <v>525</v>
       </c>
@@ -10706,7 +10721,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="63" t="s">
         <v>525</v>
       </c>
@@ -10753,7 +10768,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="63" t="s">
         <v>525</v>
       </c>
@@ -10800,7 +10815,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="s">
         <v>525</v>
       </c>
@@ -10843,7 +10858,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
         <v>525</v>
       </c>
@@ -10886,7 +10901,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
         <v>525</v>
       </c>
@@ -10933,7 +10948,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="s">
         <v>525</v>
       </c>
@@ -10980,7 +10995,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
         <v>525</v>
       </c>
@@ -11027,7 +11042,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="63" t="s">
         <v>525</v>
       </c>
@@ -11074,7 +11089,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="63" t="s">
         <v>525</v>
       </c>
@@ -11121,7 +11136,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="63" t="s">
         <v>525</v>
       </c>
@@ -11168,7 +11183,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="63" t="s">
         <v>525</v>
       </c>
@@ -11215,7 +11230,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="63" t="s">
         <v>525</v>
       </c>
@@ -11262,7 +11277,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="63" t="s">
         <v>525</v>
       </c>
@@ -11305,7 +11320,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="63" t="s">
         <v>525</v>
       </c>
@@ -11348,7 +11363,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="63" t="s">
         <v>525</v>
       </c>
@@ -11395,7 +11410,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="63" t="s">
         <v>525</v>
       </c>
@@ -11442,7 +11457,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="63" t="s">
         <v>525</v>
       </c>
@@ -11489,7 +11504,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="63" t="s">
         <v>525</v>
       </c>
@@ -11536,7 +11551,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="63" t="s">
         <v>525</v>
       </c>
@@ -11583,7 +11598,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="63" t="s">
         <v>525</v>
       </c>
@@ -11630,7 +11645,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="63" t="s">
         <v>525</v>
       </c>
@@ -11677,7 +11692,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="63" t="s">
         <v>525</v>
       </c>
@@ -11724,7 +11739,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="63" t="s">
         <v>525</v>
       </c>
@@ -11767,7 +11782,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="63" t="s">
         <v>525</v>
       </c>
@@ -11810,7 +11825,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="63" t="s">
         <v>525</v>
       </c>
@@ -11857,7 +11872,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="63" t="s">
         <v>525</v>
       </c>
@@ -11904,7 +11919,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="63" t="s">
         <v>525</v>
       </c>
@@ -11951,7 +11966,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="63" t="s">
         <v>525</v>
       </c>
@@ -11998,7 +12013,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="63" t="s">
         <v>525</v>
       </c>
@@ -12045,7 +12060,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="63" t="s">
         <v>525</v>
       </c>
@@ -12092,7 +12107,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="63" t="s">
         <v>525</v>
       </c>
@@ -12139,7 +12154,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="63" t="s">
         <v>525</v>
       </c>
@@ -12186,7 +12201,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="63" t="s">
         <v>525</v>
       </c>
@@ -12229,7 +12244,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="63" t="s">
         <v>525</v>
       </c>
@@ -12272,7 +12287,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="63" t="s">
         <v>525</v>
       </c>
@@ -12319,7 +12334,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="63" t="s">
         <v>525</v>
       </c>
@@ -12366,7 +12381,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="63" t="s">
         <v>525</v>
       </c>
@@ -12413,7 +12428,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="63" t="s">
         <v>525</v>
       </c>
@@ -12460,7 +12475,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="63" t="s">
         <v>525</v>
       </c>
@@ -12507,7 +12522,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="63" t="s">
         <v>525</v>
       </c>
@@ -12554,7 +12569,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="63" t="s">
         <v>525</v>
       </c>
@@ -12601,7 +12616,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="63" t="s">
         <v>525</v>
       </c>
@@ -12648,7 +12663,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="63" t="s">
         <v>525</v>
       </c>
@@ -12691,7 +12706,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="63" t="s">
         <v>525</v>
       </c>
@@ -12734,7 +12749,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="63" t="s">
         <v>525</v>
       </c>
@@ -12781,7 +12796,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="63" t="s">
         <v>525</v>
       </c>
@@ -12828,7 +12843,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="63" t="s">
         <v>525</v>
       </c>
@@ -12875,7 +12890,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="63" t="s">
         <v>525</v>
       </c>
@@ -12922,7 +12937,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="63" t="s">
         <v>525</v>
       </c>
@@ -12969,7 +12984,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="63" t="s">
         <v>525</v>
       </c>
@@ -13016,7 +13031,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="63" t="s">
         <v>525</v>
       </c>
@@ -13063,7 +13078,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="63" t="s">
         <v>525</v>
       </c>
@@ -13110,7 +13125,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="63" t="s">
         <v>525</v>
       </c>
@@ -13153,7 +13168,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="63" t="s">
         <v>525</v>
       </c>
@@ -13203,14 +13218,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
@@ -13224,7 +13239,7 @@
     <col min="15" max="15" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>41</v>
       </c>
@@ -13271,7 +13286,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>525</v>
       </c>
@@ -13318,7 +13333,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>525</v>
       </c>
@@ -13365,7 +13380,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>525</v>
       </c>
@@ -13412,7 +13427,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>525</v>
       </c>
@@ -13459,7 +13474,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>525</v>
       </c>
@@ -13506,7 +13521,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>525</v>
       </c>
@@ -13553,7 +13568,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>525</v>
       </c>
@@ -13600,7 +13615,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>525</v>
       </c>
@@ -13647,7 +13662,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>525</v>
       </c>
@@ -13694,7 +13709,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>525</v>
       </c>
@@ -13741,7 +13756,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="26.25">
+    <row r="12" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>525</v>
       </c>
@@ -13788,7 +13803,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="26.25">
+    <row r="13" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>525</v>
       </c>
@@ -13835,7 +13850,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="26.25">
+    <row r="14" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>525</v>
       </c>
@@ -13882,7 +13897,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="26.25">
+    <row r="15" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>525</v>
       </c>
@@ -13929,7 +13944,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="26.25">
+    <row r="16" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>525</v>
       </c>
@@ -13976,7 +13991,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="26.25">
+    <row r="17" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>525</v>
       </c>
@@ -14023,7 +14038,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="26.25">
+    <row r="18" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>525</v>
       </c>
@@ -14070,7 +14085,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="26.25">
+    <row r="19" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>525</v>
       </c>
@@ -14117,7 +14132,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="26.25">
+    <row r="20" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>525</v>
       </c>
@@ -14164,7 +14179,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="26.25">
+    <row r="21" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>525</v>
       </c>
@@ -14211,7 +14226,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="26.25">
+    <row r="22" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
         <v>525</v>
       </c>
@@ -14258,7 +14273,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="26.25">
+    <row r="23" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="62" t="s">
         <v>525</v>
       </c>
@@ -14305,7 +14320,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="26.25">
+    <row r="24" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>525</v>
       </c>
@@ -14352,7 +14367,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="26.25">
+    <row r="25" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>525</v>
       </c>
@@ -14399,7 +14414,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="26.25">
+    <row r="26" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
         <v>525</v>
       </c>
@@ -14446,7 +14461,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="26.25">
+    <row r="27" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="62" t="s">
         <v>525</v>
       </c>
@@ -14493,7 +14508,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="26.25">
+    <row r="28" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
         <v>525</v>
       </c>
@@ -14540,7 +14555,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="26.25">
+    <row r="29" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="62" t="s">
         <v>525</v>
       </c>
@@ -14587,7 +14602,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="26.25">
+    <row r="30" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="s">
         <v>525</v>
       </c>
@@ -14634,7 +14649,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="26.25">
+    <row r="31" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
         <v>525</v>
       </c>
@@ -14681,7 +14696,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="26.25">
+    <row r="32" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="s">
         <v>525</v>
       </c>
@@ -14728,7 +14743,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="26.25">
+    <row r="33" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
         <v>525</v>
       </c>
@@ -14775,7 +14790,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="26.25">
+    <row r="34" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="s">
         <v>525</v>
       </c>
@@ -14822,7 +14837,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="26.25">
+    <row r="35" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="s">
         <v>525</v>
       </c>
@@ -14869,7 +14884,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="26.25">
+    <row r="36" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="s">
         <v>525</v>
       </c>
@@ -14916,7 +14931,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="26.25">
+    <row r="37" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
         <v>525</v>
       </c>
@@ -14963,7 +14978,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="26.25">
+    <row r="38" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="62" t="s">
         <v>525</v>
       </c>
@@ -15010,7 +15025,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="26.25">
+    <row r="39" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="62" t="s">
         <v>525</v>
       </c>
@@ -15057,7 +15072,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="26.25">
+    <row r="40" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="62" t="s">
         <v>525</v>
       </c>
@@ -15104,7 +15119,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="26.25">
+    <row r="41" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="s">
         <v>525</v>
       </c>
@@ -15151,7 +15166,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="26.25">
+    <row r="42" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
         <v>525</v>
       </c>
@@ -15198,7 +15213,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="26.25">
+    <row r="43" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="62" t="s">
         <v>525</v>
       </c>
@@ -15245,7 +15260,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="26.25">
+    <row r="44" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="62" t="s">
         <v>525</v>
       </c>
@@ -15292,7 +15307,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="26.25">
+    <row r="45" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A45" s="62" t="s">
         <v>525</v>
       </c>
@@ -15339,7 +15354,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="26.25">
+    <row r="46" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A46" s="62" t="s">
         <v>525</v>
       </c>
@@ -15386,7 +15401,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="26.25">
+    <row r="47" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="62" t="s">
         <v>525</v>
       </c>
@@ -15433,7 +15448,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="26.25">
+    <row r="48" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="62" t="s">
         <v>525</v>
       </c>
@@ -15480,7 +15495,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="26.25">
+    <row r="49" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="62" t="s">
         <v>525</v>
       </c>
@@ -15527,7 +15542,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="26.25">
+    <row r="50" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="62" t="s">
         <v>525</v>
       </c>
@@ -15574,7 +15589,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="26.25">
+    <row r="51" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="62" t="s">
         <v>525</v>
       </c>
@@ -15621,7 +15636,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="26.25">
+    <row r="52" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A52" s="62" t="s">
         <v>525</v>
       </c>
@@ -15668,7 +15683,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="26.25">
+    <row r="53" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A53" s="62" t="s">
         <v>525</v>
       </c>
@@ -15715,7 +15730,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="26.25">
+    <row r="54" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A54" s="62" t="s">
         <v>525</v>
       </c>
@@ -15762,7 +15777,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="26.25">
+    <row r="55" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="62" t="s">
         <v>525</v>
       </c>
@@ -15809,7 +15824,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="26.25">
+    <row r="56" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A56" s="62" t="s">
         <v>525</v>
       </c>
@@ -15856,7 +15871,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="26.25">
+    <row r="57" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A57" s="62" t="s">
         <v>525</v>
       </c>
@@ -15903,7 +15918,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="26.25">
+    <row r="58" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A58" s="62" t="s">
         <v>525</v>
       </c>
@@ -15950,7 +15965,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="26.25">
+    <row r="59" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A59" s="62" t="s">
         <v>525</v>
       </c>
@@ -15997,7 +16012,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="26.25">
+    <row r="60" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A60" s="62" t="s">
         <v>525</v>
       </c>
@@ -16044,7 +16059,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="26.25">
+    <row r="61" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A61" s="62" t="s">
         <v>525</v>
       </c>
@@ -16091,7 +16106,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="26.25">
+    <row r="62" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A62" s="62" t="s">
         <v>525</v>
       </c>
@@ -16138,7 +16153,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="26.25">
+    <row r="63" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A63" s="62" t="s">
         <v>525</v>
       </c>
@@ -16185,7 +16200,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="26.25">
+    <row r="64" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A64" s="62" t="s">
         <v>525</v>
       </c>
@@ -16232,7 +16247,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="26.25">
+    <row r="65" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="62" t="s">
         <v>525</v>
       </c>
@@ -16279,7 +16294,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="26.25">
+    <row r="66" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="62" t="s">
         <v>525</v>
       </c>
@@ -16326,7 +16341,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="39">
+    <row r="67" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A67" s="62" t="s">
         <v>525</v>
       </c>
@@ -16373,7 +16388,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="39">
+    <row r="68" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A68" s="62" t="s">
         <v>525</v>
       </c>
@@ -16420,7 +16435,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="39">
+    <row r="69" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A69" s="62" t="s">
         <v>525</v>
       </c>
@@ -16467,7 +16482,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="39">
+    <row r="70" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A70" s="62" t="s">
         <v>525</v>
       </c>
@@ -16514,7 +16529,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="39">
+    <row r="71" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A71" s="62" t="s">
         <v>525</v>
       </c>
@@ -16561,7 +16576,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="62" t="s">
         <v>525</v>
       </c>
@@ -16608,7 +16623,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="62" t="s">
         <v>525</v>
       </c>
@@ -16655,7 +16670,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="62" t="s">
         <v>525</v>
       </c>
@@ -16702,7 +16717,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="62" t="s">
         <v>525</v>
       </c>
@@ -16749,7 +16764,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="62" t="s">
         <v>525</v>
       </c>
@@ -16796,7 +16811,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="26.25">
+    <row r="77" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="62" t="s">
         <v>525</v>
       </c>
@@ -16843,7 +16858,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="26.25">
+    <row r="78" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A78" s="62" t="s">
         <v>525</v>
       </c>
@@ -16890,7 +16905,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="26.25">
+    <row r="79" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A79" s="62" t="s">
         <v>525</v>
       </c>
@@ -16937,7 +16952,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="26.25">
+    <row r="80" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A80" s="62" t="s">
         <v>525</v>
       </c>
@@ -16984,7 +16999,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="26.25">
+    <row r="81" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A81" s="62" t="s">
         <v>525</v>
       </c>
@@ -17038,14 +17053,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="58" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -17058,7 +17073,7 @@
     <col min="15" max="15" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>41</v>
       </c>
@@ -17105,7 +17120,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="26.25">
+    <row r="2" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>525</v>
       </c>
@@ -17152,7 +17167,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="26.25">
+    <row r="3" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>525</v>
       </c>
@@ -17199,7 +17214,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="26.25">
+    <row r="4" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>525</v>
       </c>
@@ -17246,7 +17261,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>525</v>
       </c>
@@ -17293,7 +17308,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="26.25">
+    <row r="6" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>525</v>
       </c>
@@ -17340,7 +17355,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="39">
+    <row r="7" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>525</v>
       </c>
@@ -17387,7 +17402,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="39">
+    <row r="8" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>525</v>
       </c>
@@ -17434,7 +17449,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="39">
+    <row r="9" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>525</v>
       </c>
@@ -17481,7 +17496,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="39">
+    <row r="10" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>525</v>
       </c>
@@ -17528,7 +17543,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="39">
+    <row r="11" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>525</v>
       </c>
@@ -17575,7 +17590,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="26.25">
+    <row r="12" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>525</v>
       </c>
@@ -17622,7 +17637,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="26.25">
+    <row r="13" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>525</v>
       </c>
@@ -17669,7 +17684,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="26.25">
+    <row r="14" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>525</v>
       </c>
@@ -17716,7 +17731,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>525</v>
       </c>
@@ -17763,7 +17778,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="26.25">
+    <row r="16" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>525</v>
       </c>
@@ -17810,7 +17825,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="26.25">
+    <row r="17" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>525</v>
       </c>
@@ -17857,7 +17872,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="26.25">
+    <row r="18" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>525</v>
       </c>
@@ -17904,7 +17919,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="26.25">
+    <row r="19" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>525</v>
       </c>
@@ -17951,7 +17966,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="26.25">
+    <row r="20" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>525</v>
       </c>
@@ -17998,7 +18013,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="26.25">
+    <row r="21" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>525</v>
       </c>
@@ -18051,14 +18066,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -18077,7 +18092,7 @@
     <col min="16" max="16" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
         <v>41</v>
       </c>
@@ -18127,7 +18142,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>525</v>
       </c>
@@ -18177,7 +18192,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>525</v>
       </c>
@@ -18227,7 +18242,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>525</v>
       </c>
@@ -18277,7 +18292,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>525</v>
       </c>
@@ -18327,7 +18342,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>525</v>
       </c>
@@ -18377,7 +18392,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>525</v>
       </c>
@@ -18427,7 +18442,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>525</v>
       </c>
@@ -18477,7 +18492,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>525</v>
       </c>
@@ -18527,7 +18542,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>525</v>
       </c>
@@ -18577,7 +18592,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>525</v>
       </c>
@@ -18627,7 +18642,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="62" t="s">
         <v>525</v>
       </c>
@@ -18677,7 +18692,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>525</v>
       </c>
@@ -18727,7 +18742,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>525</v>
       </c>
@@ -18777,7 +18792,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>525</v>
       </c>
@@ -18827,7 +18842,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="62" t="s">
         <v>525</v>
       </c>
@@ -18877,7 +18892,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>525</v>
       </c>
@@ -18927,7 +18942,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>525</v>
       </c>
@@ -18977,7 +18992,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="39">
+    <row r="19" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>525</v>
       </c>
@@ -19027,7 +19042,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="39">
+    <row r="20" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>525</v>
       </c>
@@ -19077,7 +19092,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="39">
+    <row r="21" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>525</v>
       </c>
@@ -19127,7 +19142,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="39">
+    <row r="22" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
         <v>525</v>
       </c>
@@ -19177,7 +19192,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="39">
+    <row r="23" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="62" t="s">
         <v>525</v>
       </c>
@@ -19227,7 +19242,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="39">
+    <row r="24" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>525</v>
       </c>
@@ -19277,7 +19292,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="39">
+    <row r="25" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>525</v>
       </c>
@@ -19327,7 +19342,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="26.25">
+    <row r="26" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
         <v>525</v>
       </c>
@@ -19377,7 +19392,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="39">
+    <row r="27" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A27" s="62" t="s">
         <v>525</v>
       </c>
@@ -19427,7 +19442,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="39">
+    <row r="28" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
         <v>525</v>
       </c>
@@ -19477,7 +19492,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="39">
+    <row r="29" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="62" t="s">
         <v>525</v>
       </c>
@@ -19527,7 +19542,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="s">
         <v>525</v>
       </c>
@@ -19577,7 +19592,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
         <v>525</v>
       </c>
@@ -19627,7 +19642,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="s">
         <v>525</v>
       </c>
@@ -19677,7 +19692,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
         <v>525</v>
       </c>
@@ -19727,7 +19742,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="s">
         <v>525</v>
       </c>
@@ -19777,7 +19792,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="s">
         <v>525</v>
       </c>
@@ -19827,7 +19842,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="s">
         <v>525</v>
       </c>
@@ -19877,7 +19892,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
         <v>525</v>
       </c>
@@ -19927,7 +19942,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="62" t="s">
         <v>525</v>
       </c>
@@ -19977,7 +19992,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="39">
+    <row r="39" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A39" s="62" t="s">
         <v>525</v>
       </c>
@@ -20027,7 +20042,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="39">
+    <row r="40" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A40" s="62" t="s">
         <v>525</v>
       </c>
@@ -20077,7 +20092,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="39">
+    <row r="41" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="s">
         <v>525</v>
       </c>
@@ -20127,7 +20142,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="39">
+    <row r="42" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
         <v>525</v>
       </c>
@@ -20177,7 +20192,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="39">
+    <row r="43" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A43" s="62" t="s">
         <v>525</v>
       </c>
@@ -20227,7 +20242,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="39">
+    <row r="44" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A44" s="62" t="s">
         <v>525</v>
       </c>
@@ -20277,7 +20292,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="39">
+    <row r="45" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A45" s="62" t="s">
         <v>525</v>
       </c>
@@ -20327,7 +20342,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="39">
+    <row r="46" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A46" s="62" t="s">
         <v>525</v>
       </c>
@@ -20377,7 +20392,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="39">
+    <row r="47" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A47" s="62" t="s">
         <v>525</v>
       </c>
@@ -20427,7 +20442,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="26.25">
+    <row r="48" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="62" t="s">
         <v>525</v>
       </c>
@@ -20477,7 +20492,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="39">
+    <row r="49" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A49" s="62" t="s">
         <v>525</v>
       </c>
@@ -20527,7 +20542,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="39">
+    <row r="50" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A50" s="62" t="s">
         <v>525</v>
       </c>
@@ -20577,7 +20592,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="39">
+    <row r="51" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A51" s="62" t="s">
         <v>525</v>
       </c>
@@ -20627,7 +20642,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="39">
+    <row r="52" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A52" s="62" t="s">
         <v>525</v>
       </c>
@@ -20677,7 +20692,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="39">
+    <row r="53" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A53" s="62" t="s">
         <v>525</v>
       </c>
@@ -20727,7 +20742,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="39">
+    <row r="54" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A54" s="62" t="s">
         <v>525</v>
       </c>
@@ -20777,7 +20792,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="39">
+    <row r="55" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A55" s="62" t="s">
         <v>525</v>
       </c>
@@ -20827,7 +20842,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="39">
+    <row r="56" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A56" s="62" t="s">
         <v>525</v>
       </c>
@@ -20877,7 +20892,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="39">
+    <row r="57" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A57" s="62" t="s">
         <v>525</v>
       </c>
@@ -20927,7 +20942,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="39">
+    <row r="58" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A58" s="62" t="s">
         <v>525</v>
       </c>
@@ -20977,7 +20992,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="39">
+    <row r="59" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A59" s="62" t="s">
         <v>525</v>
       </c>
@@ -21027,7 +21042,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="26.25">
+    <row r="60" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A60" s="62" t="s">
         <v>525</v>
       </c>
@@ -21077,7 +21092,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="39">
+    <row r="61" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A61" s="62" t="s">
         <v>525</v>
       </c>
@@ -21127,7 +21142,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="39">
+    <row r="62" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A62" s="62" t="s">
         <v>525</v>
       </c>
@@ -21177,7 +21192,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="62"/>
       <c r="B63" s="68"/>
       <c r="C63" s="68"/>
@@ -21195,7 +21210,7 @@
       <c r="O63" s="68"/>
       <c r="P63" s="64"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="62"/>
       <c r="B64" s="62"/>
       <c r="C64" s="62"/>

</xml_diff>

<commit_message>
Commit on 14th jan 2016 new
</commit_message>
<xml_diff>
--- a/Excels/Data_QA_Tests.xlsx
+++ b/Excels/Data_QA_Tests.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sahi_pro\userdata\12twenty\excels\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="11760" tabRatio="661"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="11760" tabRatio="661" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MBA Standard Reports" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5598" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5598" uniqueCount="525">
   <si>
     <t>Site Instance</t>
   </si>
@@ -1599,16 +1594,13 @@
   </si>
   <si>
     <t xml:space="preserve">Post Graduation  </t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1949,7 +1941,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1981,10 +1973,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2016,7 +2007,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2192,14 +2182,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -2212,7 +2202,7 @@
     <col min="15" max="15" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="31.5" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>41</v>
       </c>
@@ -2259,7 +2249,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -2306,9 +2296,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -2353,9 +2343,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -2400,9 +2390,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -2447,9 +2437,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -2494,9 +2484,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -2541,9 +2531,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>9</v>
@@ -2588,9 +2578,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>9</v>
@@ -2635,9 +2625,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>9</v>
@@ -2682,9 +2672,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>9</v>
@@ -2729,9 +2719,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
@@ -2776,9 +2766,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -2823,9 +2813,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
@@ -2870,9 +2860,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
@@ -2917,9 +2907,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
@@ -2964,9 +2954,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
@@ -3011,9 +3001,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
@@ -3058,9 +3048,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
@@ -3105,9 +3095,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>9</v>
@@ -3152,9 +3142,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>9</v>
@@ -3199,9 +3189,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>9</v>
@@ -3246,9 +3236,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>9</v>
@@ -3293,9 +3283,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>9</v>
@@ -3340,9 +3330,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>9</v>
@@ -3387,9 +3377,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>9</v>
@@ -3434,9 +3424,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>9</v>
@@ -3481,9 +3471,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>9</v>
@@ -3528,9 +3518,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>9</v>
@@ -3575,9 +3565,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>9</v>
@@ -3622,9 +3612,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>9</v>
@@ -3669,9 +3659,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>9</v>
@@ -3716,9 +3706,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>9</v>
@@ -3763,9 +3753,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>9</v>
@@ -3810,9 +3800,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>9</v>
@@ -3857,9 +3847,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>9</v>
@@ -3904,9 +3894,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>9</v>
@@ -3951,9 +3941,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>9</v>
@@ -3998,9 +3988,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>9</v>
@@ -4045,9 +4035,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>9</v>
@@ -4092,9 +4082,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>9</v>
@@ -4139,9 +4129,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="26.25">
       <c r="A42" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>9</v>
@@ -4186,9 +4176,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="26.25">
       <c r="A43" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>9</v>
@@ -4233,9 +4223,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="26.25">
       <c r="A44" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>9</v>
@@ -4280,9 +4270,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="26.25">
       <c r="A45" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>9</v>
@@ -4327,9 +4317,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="26.25">
       <c r="A46" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>9</v>
@@ -4374,9 +4364,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="26.25">
       <c r="A47" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>9</v>
@@ -4421,9 +4411,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="26.25">
       <c r="A48" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>9</v>
@@ -4468,9 +4458,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="26.25">
       <c r="A49" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>9</v>
@@ -4515,9 +4505,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="26.25">
       <c r="A50" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>9</v>
@@ -4562,9 +4552,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="26.25">
       <c r="A51" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>9</v>
@@ -4609,9 +4599,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>9</v>
@@ -4656,9 +4646,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>9</v>
@@ -4703,9 +4693,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>9</v>
@@ -4750,9 +4740,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>9</v>
@@ -4797,9 +4787,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="A56" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>9</v>
@@ -4844,9 +4834,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>9</v>
@@ -4891,9 +4881,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>9</v>
@@ -4938,9 +4928,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15">
       <c r="A59" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>9</v>
@@ -4985,9 +4975,9 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15">
       <c r="A60" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>9</v>
@@ -5032,9 +5022,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B61" s="19" t="s">
         <v>9</v>
@@ -5079,9 +5069,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="26.25">
       <c r="A62" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>9</v>
@@ -5126,9 +5116,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="26.25">
       <c r="A63" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>9</v>
@@ -5173,9 +5163,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="26.25">
       <c r="A64" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>9</v>
@@ -5220,9 +5210,9 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="26.25">
       <c r="A65" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>9</v>
@@ -5267,9 +5257,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="26.25">
       <c r="A66" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>9</v>
@@ -5314,9 +5304,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="26.25">
       <c r="A67" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>9</v>
@@ -5361,9 +5351,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="26.25">
       <c r="A68" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>9</v>
@@ -5408,9 +5398,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="26.25">
       <c r="A69" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>9</v>
@@ -5455,9 +5445,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="26.25">
       <c r="A70" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>9</v>
@@ -5502,9 +5492,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="26.25">
       <c r="A71" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>9</v>
@@ -5549,9 +5539,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15">
       <c r="A72" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>9</v>
@@ -5596,9 +5586,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15">
       <c r="A73" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>9</v>
@@ -5643,9 +5633,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15">
       <c r="A74" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
@@ -5690,9 +5680,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
@@ -5737,9 +5727,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15">
       <c r="A76" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>9</v>
@@ -5784,9 +5774,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15">
       <c r="A77" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>9</v>
@@ -5831,9 +5821,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15">
       <c r="A78" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>9</v>
@@ -5878,9 +5868,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15">
       <c r="A79" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>9</v>
@@ -5925,9 +5915,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15">
       <c r="A80" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>9</v>
@@ -5972,9 +5962,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15">
       <c r="A81" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>9</v>
@@ -6019,9 +6009,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15">
       <c r="A82" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>9</v>
@@ -6066,9 +6056,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15">
       <c r="A83" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>9</v>
@@ -6113,9 +6103,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15">
       <c r="A84" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>9</v>
@@ -6160,9 +6150,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15">
       <c r="A85" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>9</v>
@@ -6207,9 +6197,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15">
       <c r="A86" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>9</v>
@@ -6254,9 +6244,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15">
       <c r="A87" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>9</v>
@@ -6301,9 +6291,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15">
       <c r="A88" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>9</v>
@@ -6348,9 +6338,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15">
       <c r="A89" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>9</v>
@@ -6395,9 +6385,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15">
       <c r="A90" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>9</v>
@@ -6442,9 +6432,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15">
       <c r="A91" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>9</v>
@@ -6489,9 +6479,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="26.25">
       <c r="A92" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>9</v>
@@ -6536,9 +6526,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="26.25">
       <c r="A93" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>9</v>
@@ -6583,9 +6573,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="26.25">
       <c r="A94" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>9</v>
@@ -6630,9 +6620,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="26.25">
       <c r="A95" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>9</v>
@@ -6677,9 +6667,9 @@
         <v>163</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="26.25">
       <c r="A96" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>9</v>
@@ -6724,9 +6714,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="26.25">
       <c r="A97" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>9</v>
@@ -6771,9 +6761,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="26.25">
       <c r="A98" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>9</v>
@@ -6818,9 +6808,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="26.25">
       <c r="A99" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>9</v>
@@ -6865,9 +6855,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="26.25">
       <c r="A100" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>9</v>
@@ -6912,9 +6902,9 @@
         <v>168</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="26.25">
       <c r="A101" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B101" s="19" t="s">
         <v>9</v>
@@ -6959,9 +6949,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="26.25">
       <c r="A102" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>9</v>
@@ -7006,9 +6996,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="26.25">
       <c r="A103" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>9</v>
@@ -7053,9 +7043,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="26.25">
       <c r="A104" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>9</v>
@@ -7100,9 +7090,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="26.25">
       <c r="A105" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>9</v>
@@ -7147,9 +7137,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="26.25">
       <c r="A106" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>9</v>
@@ -7194,9 +7184,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="26.25">
       <c r="A107" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>9</v>
@@ -7241,9 +7231,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="26.25">
       <c r="A108" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>9</v>
@@ -7288,9 +7278,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="26.25">
       <c r="A109" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>9</v>
@@ -7335,9 +7325,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="26.25">
       <c r="A110" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>9</v>
@@ -7382,9 +7372,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="26.25">
       <c r="A111" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B111" s="19" t="s">
         <v>9</v>
@@ -7429,9 +7419,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="26.25">
       <c r="A112" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>9</v>
@@ -7476,9 +7466,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="26.25">
       <c r="A113" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>9</v>
@@ -7523,9 +7513,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="26.25">
       <c r="A114" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>9</v>
@@ -7570,9 +7560,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="26.25">
       <c r="A115" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>9</v>
@@ -7617,9 +7607,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="26.25">
       <c r="A116" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>9</v>
@@ -7664,9 +7654,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="26.25">
       <c r="A117" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>9</v>
@@ -7711,9 +7701,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="26.25">
       <c r="A118" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>9</v>
@@ -7758,9 +7748,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="26.25">
       <c r="A119" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>9</v>
@@ -7805,9 +7795,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="26.25">
       <c r="A120" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>9</v>
@@ -7852,9 +7842,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="26.25">
       <c r="A121" s="1" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B121" s="19" t="s">
         <v>9</v>
@@ -7906,14 +7896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -7928,7 +7918,7 @@
     <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="31.5" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>41</v>
       </c>
@@ -7976,9 +7966,9 @@
       </c>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>19</v>
@@ -8024,9 +8014,9 @@
       </c>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>19</v>
@@ -8072,9 +8062,9 @@
       </c>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>19</v>
@@ -8120,9 +8110,9 @@
       </c>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>19</v>
@@ -8168,9 +8158,9 @@
       </c>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>19</v>
@@ -8216,9 +8206,9 @@
       </c>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>19</v>
@@ -8264,9 +8254,9 @@
       </c>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>19</v>
@@ -8312,9 +8302,9 @@
       </c>
       <c r="P8" s="13"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>19</v>
@@ -8360,9 +8350,9 @@
       </c>
       <c r="P9" s="13"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>19</v>
@@ -8408,9 +8398,9 @@
       </c>
       <c r="P10" s="13"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>19</v>
@@ -8456,9 +8446,9 @@
       </c>
       <c r="P11" s="13"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>19</v>
@@ -8504,9 +8494,9 @@
       </c>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>19</v>
@@ -8552,9 +8542,9 @@
       </c>
       <c r="P13" s="13"/>
     </row>
-    <row r="14" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="26.25">
       <c r="A14" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>19</v>
@@ -8600,9 +8590,9 @@
       </c>
       <c r="P14" s="13"/>
     </row>
-    <row r="15" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="26.25">
       <c r="A15" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>19</v>
@@ -8648,9 +8638,9 @@
       </c>
       <c r="P15" s="13"/>
     </row>
-    <row r="16" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="26.25">
       <c r="A16" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>19</v>
@@ -8696,9 +8686,9 @@
       </c>
       <c r="P16" s="13"/>
     </row>
-    <row r="17" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="26.25">
       <c r="A17" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>19</v>
@@ -8744,9 +8734,9 @@
       </c>
       <c r="P17" s="13"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>19</v>
@@ -8792,9 +8782,9 @@
       </c>
       <c r="P18" s="13"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>19</v>
@@ -8840,9 +8830,9 @@
       </c>
       <c r="P19" s="13"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>19</v>
@@ -8888,9 +8878,9 @@
       </c>
       <c r="P20" s="13"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>19</v>
@@ -8936,9 +8926,9 @@
       </c>
       <c r="P21" s="13"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>19</v>
@@ -8984,9 +8974,9 @@
       </c>
       <c r="P22" s="13"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>19</v>
@@ -9032,9 +9022,9 @@
       </c>
       <c r="P23" s="13"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>19</v>
@@ -9080,9 +9070,9 @@
       </c>
       <c r="P24" s="13"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>19</v>
@@ -9128,9 +9118,9 @@
       </c>
       <c r="P25" s="13"/>
     </row>
-    <row r="26" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="26.25">
       <c r="A26" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>19</v>
@@ -9176,9 +9166,9 @@
       </c>
       <c r="P26" s="13"/>
     </row>
-    <row r="27" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="26.25">
       <c r="A27" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>19</v>
@@ -9224,9 +9214,9 @@
       </c>
       <c r="P27" s="13"/>
     </row>
-    <row r="28" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="26.25">
       <c r="A28" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>19</v>
@@ -9272,9 +9262,9 @@
       </c>
       <c r="P28" s="13"/>
     </row>
-    <row r="29" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="26.25">
       <c r="A29" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>19</v>
@@ -9320,9 +9310,9 @@
       </c>
       <c r="P29" s="13"/>
     </row>
-    <row r="30" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="26.25">
       <c r="A30" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>19</v>
@@ -9368,9 +9358,9 @@
       </c>
       <c r="P30" s="13"/>
     </row>
-    <row r="31" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="26.25">
       <c r="A31" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>19</v>
@@ -9416,9 +9406,9 @@
       </c>
       <c r="P31" s="13"/>
     </row>
-    <row r="32" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="26.25">
       <c r="A32" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>19</v>
@@ -9464,9 +9454,9 @@
       </c>
       <c r="P32" s="13"/>
     </row>
-    <row r="33" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="26.25">
       <c r="A33" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>19</v>
@@ -9512,9 +9502,9 @@
       </c>
       <c r="P33" s="13"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>19</v>
@@ -9560,7 +9550,7 @@
       </c>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" s="62" t="s">
         <v>42</v>
       </c>
@@ -9608,7 +9598,7 @@
       </c>
       <c r="P35" s="13"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" s="62" t="s">
         <v>42</v>
       </c>
@@ -9656,7 +9646,7 @@
       </c>
       <c r="P36" s="13"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" s="62" t="s">
         <v>42</v>
       </c>
@@ -9704,7 +9694,7 @@
       </c>
       <c r="P37" s="13"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="62" t="s">
         <v>42</v>
       </c>
@@ -9752,9 +9742,9 @@
       </c>
       <c r="P38" s="13"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>19</v>
@@ -9800,9 +9790,9 @@
       </c>
       <c r="P39" s="13"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>19</v>
@@ -9848,9 +9838,9 @@
       </c>
       <c r="P40" s="13"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>19</v>
@@ -9903,14 +9893,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
@@ -9929,7 +9919,7 @@
     <col min="15" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="37.5" customHeight="1">
       <c r="A1" s="65" t="s">
         <v>41</v>
       </c>
@@ -9977,9 +9967,9 @@
       </c>
       <c r="P1" s="66"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>20</v>
@@ -10024,9 +10014,9 @@
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>20</v>
@@ -10071,9 +10061,9 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B4" s="63" t="s">
         <v>20</v>
@@ -10118,9 +10108,9 @@
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B5" s="63" t="s">
         <v>20</v>
@@ -10165,9 +10155,9 @@
         <v>361</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B6" s="63" t="s">
         <v>20</v>
@@ -10212,9 +10202,9 @@
         <v>362</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B7" s="63" t="s">
         <v>20</v>
@@ -10259,9 +10249,9 @@
         <v>363</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B8" s="63" t="s">
         <v>20</v>
@@ -10306,9 +10296,9 @@
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B9" s="63" t="s">
         <v>20</v>
@@ -10353,9 +10343,9 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B10" s="63" t="s">
         <v>20</v>
@@ -10396,9 +10386,9 @@
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B11" s="63" t="s">
         <v>20</v>
@@ -10439,9 +10429,9 @@
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B12" s="63" t="s">
         <v>20</v>
@@ -10486,9 +10476,9 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B13" s="63" t="s">
         <v>20</v>
@@ -10533,9 +10523,9 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B14" s="63" t="s">
         <v>20</v>
@@ -10580,9 +10570,9 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B15" s="63" t="s">
         <v>20</v>
@@ -10627,9 +10617,9 @@
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B16" s="63" t="s">
         <v>20</v>
@@ -10674,9 +10664,9 @@
         <v>374</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B17" s="63" t="s">
         <v>20</v>
@@ -10721,9 +10711,9 @@
         <v>375</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B18" s="63" t="s">
         <v>20</v>
@@ -10768,9 +10758,9 @@
         <v>376</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B19" s="63" t="s">
         <v>20</v>
@@ -10815,9 +10805,9 @@
         <v>377</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B20" s="63" t="s">
         <v>20</v>
@@ -10858,9 +10848,9 @@
         <v>378</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B21" s="63" t="s">
         <v>20</v>
@@ -10901,9 +10891,9 @@
         <v>379</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B22" s="63" t="s">
         <v>20</v>
@@ -10948,9 +10938,9 @@
         <v>381</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B23" s="63" t="s">
         <v>20</v>
@@ -10995,9 +10985,9 @@
         <v>382</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B24" s="63" t="s">
         <v>20</v>
@@ -11042,9 +11032,9 @@
         <v>383</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B25" s="63" t="s">
         <v>20</v>
@@ -11089,9 +11079,9 @@
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B26" s="63" t="s">
         <v>20</v>
@@ -11136,9 +11126,9 @@
         <v>385</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B27" s="63" t="s">
         <v>20</v>
@@ -11183,9 +11173,9 @@
         <v>386</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B28" s="63" t="s">
         <v>20</v>
@@ -11230,9 +11220,9 @@
         <v>387</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B29" s="63" t="s">
         <v>20</v>
@@ -11277,9 +11267,9 @@
         <v>388</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B30" s="63" t="s">
         <v>20</v>
@@ -11320,9 +11310,9 @@
         <v>389</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B31" s="63" t="s">
         <v>20</v>
@@ -11363,9 +11353,9 @@
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B32" s="63" t="s">
         <v>20</v>
@@ -11410,9 +11400,9 @@
         <v>392</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B33" s="63" t="s">
         <v>20</v>
@@ -11457,9 +11447,9 @@
         <v>393</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B34" s="63" t="s">
         <v>20</v>
@@ -11504,9 +11494,9 @@
         <v>394</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B35" s="63" t="s">
         <v>20</v>
@@ -11551,9 +11541,9 @@
         <v>395</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B36" s="63" t="s">
         <v>20</v>
@@ -11598,9 +11588,9 @@
         <v>396</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B37" s="63" t="s">
         <v>20</v>
@@ -11645,9 +11635,9 @@
         <v>397</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B38" s="63" t="s">
         <v>20</v>
@@ -11692,9 +11682,9 @@
         <v>398</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B39" s="63" t="s">
         <v>20</v>
@@ -11739,9 +11729,9 @@
         <v>399</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B40" s="63" t="s">
         <v>20</v>
@@ -11782,9 +11772,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B41" s="63" t="s">
         <v>20</v>
@@ -11825,9 +11815,9 @@
         <v>401</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B42" s="63" t="s">
         <v>20</v>
@@ -11872,9 +11862,9 @@
         <v>403</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B43" s="63" t="s">
         <v>20</v>
@@ -11919,9 +11909,9 @@
         <v>404</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B44" s="63" t="s">
         <v>20</v>
@@ -11966,9 +11956,9 @@
         <v>405</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B45" s="63" t="s">
         <v>20</v>
@@ -12013,9 +12003,9 @@
         <v>406</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B46" s="63" t="s">
         <v>20</v>
@@ -12060,9 +12050,9 @@
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B47" s="63" t="s">
         <v>20</v>
@@ -12107,9 +12097,9 @@
         <v>408</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B48" s="63" t="s">
         <v>20</v>
@@ -12154,9 +12144,9 @@
         <v>409</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B49" s="63" t="s">
         <v>20</v>
@@ -12201,9 +12191,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B50" s="63" t="s">
         <v>20</v>
@@ -12244,9 +12234,9 @@
         <v>411</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B51" s="63" t="s">
         <v>20</v>
@@ -12287,9 +12277,9 @@
         <v>412</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B52" s="63" t="s">
         <v>20</v>
@@ -12334,9 +12324,9 @@
         <v>414</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B53" s="63" t="s">
         <v>20</v>
@@ -12381,9 +12371,9 @@
         <v>415</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B54" s="63" t="s">
         <v>20</v>
@@ -12428,9 +12418,9 @@
         <v>416</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B55" s="63" t="s">
         <v>20</v>
@@ -12475,9 +12465,9 @@
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="A56" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B56" s="63" t="s">
         <v>20</v>
@@ -12522,9 +12512,9 @@
         <v>418</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B57" s="63" t="s">
         <v>20</v>
@@ -12569,9 +12559,9 @@
         <v>419</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B58" s="63" t="s">
         <v>20</v>
@@ -12616,9 +12606,9 @@
         <v>420</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15">
       <c r="A59" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B59" s="63" t="s">
         <v>20</v>
@@ -12663,9 +12653,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15">
       <c r="A60" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B60" s="63" t="s">
         <v>20</v>
@@ -12706,9 +12696,9 @@
         <v>422</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B61" s="63" t="s">
         <v>20</v>
@@ -12749,9 +12739,9 @@
         <v>423</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15">
       <c r="A62" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B62" s="63" t="s">
         <v>20</v>
@@ -12796,9 +12786,9 @@
         <v>425</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B63" s="63" t="s">
         <v>20</v>
@@ -12843,9 +12833,9 @@
         <v>426</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B64" s="63" t="s">
         <v>20</v>
@@ -12890,9 +12880,9 @@
         <v>427</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15">
       <c r="A65" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B65" s="63" t="s">
         <v>20</v>
@@ -12937,9 +12927,9 @@
         <v>428</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B66" s="63" t="s">
         <v>20</v>
@@ -12984,9 +12974,9 @@
         <v>429</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15">
       <c r="A67" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B67" s="63" t="s">
         <v>20</v>
@@ -13031,9 +13021,9 @@
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15">
       <c r="A68" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B68" s="63" t="s">
         <v>20</v>
@@ -13078,9 +13068,9 @@
         <v>431</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15">
       <c r="A69" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B69" s="63" t="s">
         <v>20</v>
@@ -13125,9 +13115,9 @@
         <v>432</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15">
       <c r="A70" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B70" s="63" t="s">
         <v>20</v>
@@ -13168,9 +13158,9 @@
         <v>433</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15">
       <c r="A71" s="63" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B71" s="63" t="s">
         <v>20</v>
@@ -13218,14 +13208,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
@@ -13239,7 +13229,7 @@
     <col min="15" max="15" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="26.25">
       <c r="A1" s="31" t="s">
         <v>41</v>
       </c>
@@ -13286,9 +13276,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>25</v>
@@ -13333,9 +13323,9 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>25</v>
@@ -13380,9 +13370,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>25</v>
@@ -13427,9 +13417,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>25</v>
@@ -13474,9 +13464,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>25</v>
@@ -13521,9 +13511,9 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>25</v>
@@ -13568,9 +13558,9 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>25</v>
@@ -13615,9 +13605,9 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>25</v>
@@ -13662,9 +13652,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>25</v>
@@ -13709,9 +13699,9 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>25</v>
@@ -13756,9 +13746,9 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="26.25">
       <c r="A12" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>25</v>
@@ -13803,9 +13793,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="26.25">
       <c r="A13" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>25</v>
@@ -13850,9 +13840,9 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="26.25">
       <c r="A14" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>25</v>
@@ -13897,9 +13887,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="26.25">
       <c r="A15" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>25</v>
@@ -13944,9 +13934,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="26.25">
       <c r="A16" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>25</v>
@@ -13991,9 +13981,9 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="26.25">
       <c r="A17" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>25</v>
@@ -14038,9 +14028,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="26.25">
       <c r="A18" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>25</v>
@@ -14085,9 +14075,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="26.25">
       <c r="A19" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>25</v>
@@ -14132,9 +14122,9 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="26.25">
       <c r="A20" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>25</v>
@@ -14179,9 +14169,9 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="26.25">
       <c r="A21" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>25</v>
@@ -14226,9 +14216,9 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="26.25">
       <c r="A22" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>25</v>
@@ -14273,9 +14263,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="26.25">
       <c r="A23" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>25</v>
@@ -14320,9 +14310,9 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="26.25">
       <c r="A24" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>25</v>
@@ -14367,9 +14357,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="26.25">
       <c r="A25" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>25</v>
@@ -14414,9 +14404,9 @@
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="26.25">
       <c r="A26" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>25</v>
@@ -14461,9 +14451,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="26.25">
       <c r="A27" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>25</v>
@@ -14508,9 +14498,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="26.25">
       <c r="A28" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>25</v>
@@ -14555,9 +14545,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="26.25">
       <c r="A29" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>25</v>
@@ -14602,9 +14592,9 @@
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="26.25">
       <c r="A30" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>25</v>
@@ -14649,9 +14639,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="26.25">
       <c r="A31" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>25</v>
@@ -14696,9 +14686,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="26.25">
       <c r="A32" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>25</v>
@@ -14743,9 +14733,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="26.25">
       <c r="A33" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>25</v>
@@ -14790,9 +14780,9 @@
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="26.25">
       <c r="A34" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>25</v>
@@ -14837,9 +14827,9 @@
         <v>239</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="26.25">
       <c r="A35" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>25</v>
@@ -14884,9 +14874,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="26.25">
       <c r="A36" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>25</v>
@@ -14931,9 +14921,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="26.25">
       <c r="A37" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>25</v>
@@ -14978,9 +14968,9 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="26.25">
       <c r="A38" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>25</v>
@@ -15025,9 +15015,9 @@
         <v>243</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="26.25">
       <c r="A39" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>25</v>
@@ -15072,9 +15062,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="26.25">
       <c r="A40" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>25</v>
@@ -15119,9 +15109,9 @@
         <v>245</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="26.25">
       <c r="A41" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>25</v>
@@ -15166,9 +15156,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="26.25">
       <c r="A42" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>25</v>
@@ -15213,9 +15203,9 @@
         <v>247</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="26.25">
       <c r="A43" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>25</v>
@@ -15260,9 +15250,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="26.25">
       <c r="A44" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>25</v>
@@ -15307,9 +15297,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="26.25">
       <c r="A45" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>25</v>
@@ -15354,9 +15344,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="26.25">
       <c r="A46" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>25</v>
@@ -15401,9 +15391,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="26.25">
       <c r="A47" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>25</v>
@@ -15448,9 +15438,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="26.25">
       <c r="A48" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>25</v>
@@ -15495,9 +15485,9 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="26.25">
       <c r="A49" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>25</v>
@@ -15542,9 +15532,9 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="26.25">
       <c r="A50" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>25</v>
@@ -15589,9 +15579,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="26.25">
       <c r="A51" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>25</v>
@@ -15636,9 +15626,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="26.25">
       <c r="A52" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>25</v>
@@ -15683,9 +15673,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="26.25">
       <c r="A53" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>25</v>
@@ -15730,9 +15720,9 @@
         <v>258</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="26.25">
       <c r="A54" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>25</v>
@@ -15777,9 +15767,9 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="26.25">
       <c r="A55" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>25</v>
@@ -15824,9 +15814,9 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="26.25">
       <c r="A56" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>25</v>
@@ -15871,9 +15861,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="26.25">
       <c r="A57" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>25</v>
@@ -15918,9 +15908,9 @@
         <v>262</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="26.25">
       <c r="A58" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>25</v>
@@ -15965,9 +15955,9 @@
         <v>263</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="26.25">
       <c r="A59" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>25</v>
@@ -16012,9 +16002,9 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="26.25">
       <c r="A60" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>25</v>
@@ -16059,9 +16049,9 @@
         <v>265</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="26.25">
       <c r="A61" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>25</v>
@@ -16106,9 +16096,9 @@
         <v>266</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="26.25">
       <c r="A62" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>25</v>
@@ -16153,9 +16143,9 @@
         <v>267</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="26.25">
       <c r="A63" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>25</v>
@@ -16200,9 +16190,9 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="26.25">
       <c r="A64" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>25</v>
@@ -16247,9 +16237,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="26.25">
       <c r="A65" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B65" s="11" t="s">
         <v>25</v>
@@ -16294,9 +16284,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="26.25">
       <c r="A66" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>25</v>
@@ -16341,9 +16331,9 @@
         <v>271</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="39">
       <c r="A67" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>25</v>
@@ -16388,9 +16378,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="39">
       <c r="A68" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>25</v>
@@ -16435,9 +16425,9 @@
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="39">
       <c r="A69" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>25</v>
@@ -16482,9 +16472,9 @@
         <v>274</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="39">
       <c r="A70" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>25</v>
@@ -16529,9 +16519,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="39">
       <c r="A71" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>25</v>
@@ -16576,9 +16566,9 @@
         <v>276</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15">
       <c r="A72" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>25</v>
@@ -16623,9 +16613,9 @@
         <v>277</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15">
       <c r="A73" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>25</v>
@@ -16670,9 +16660,9 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15">
       <c r="A74" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>25</v>
@@ -16717,9 +16707,9 @@
         <v>279</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>25</v>
@@ -16764,9 +16754,9 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15">
       <c r="A76" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>25</v>
@@ -16811,9 +16801,9 @@
         <v>281</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="26.25">
       <c r="A77" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>25</v>
@@ -16858,9 +16848,9 @@
         <v>282</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="26.25">
       <c r="A78" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>25</v>
@@ -16905,9 +16895,9 @@
         <v>283</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="26.25">
       <c r="A79" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>25</v>
@@ -16952,9 +16942,9 @@
         <v>284</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="26.25">
       <c r="A80" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B80" s="11" t="s">
         <v>25</v>
@@ -16999,9 +16989,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="26.25">
       <c r="A81" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>25</v>
@@ -17053,14 +17043,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="58" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -17073,7 +17063,7 @@
     <col min="15" max="15" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="26.25">
       <c r="A1" s="31" t="s">
         <v>41</v>
       </c>
@@ -17120,9 +17110,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="26.25">
       <c r="A2" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
@@ -17167,9 +17157,9 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="26.25">
       <c r="A3" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>29</v>
@@ -17214,9 +17204,9 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="26.25">
       <c r="A4" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>29</v>
@@ -17261,9 +17251,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>29</v>
@@ -17308,9 +17298,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="26.25">
       <c r="A6" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>29</v>
@@ -17355,9 +17345,9 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="39">
       <c r="A7" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>29</v>
@@ -17402,9 +17392,9 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="39">
       <c r="A8" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>29</v>
@@ -17449,9 +17439,9 @@
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="39">
       <c r="A9" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>29</v>
@@ -17496,9 +17486,9 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="39">
       <c r="A10" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>29</v>
@@ -17543,9 +17533,9 @@
         <v>336</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="39">
       <c r="A11" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>29</v>
@@ -17590,9 +17580,9 @@
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="26.25">
       <c r="A12" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>29</v>
@@ -17637,9 +17627,9 @@
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="26.25">
       <c r="A13" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>29</v>
@@ -17684,9 +17674,9 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="26.25">
       <c r="A14" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>29</v>
@@ -17731,9 +17721,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>29</v>
@@ -17778,9 +17768,9 @@
         <v>341</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="26.25">
       <c r="A16" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
@@ -17825,9 +17815,9 @@
         <v>342</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="26.25">
       <c r="A17" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>29</v>
@@ -17872,9 +17862,9 @@
         <v>343</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="26.25">
       <c r="A18" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>29</v>
@@ -17919,9 +17909,9 @@
         <v>344</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="26.25">
       <c r="A19" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>29</v>
@@ -17966,9 +17956,9 @@
         <v>345</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="26.25">
       <c r="A20" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>29</v>
@@ -18013,9 +18003,9 @@
         <v>346</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="26.25">
       <c r="A21" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>29</v>
@@ -18066,14 +18056,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -18092,7 +18082,7 @@
     <col min="16" max="16" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="67" t="s">
         <v>41</v>
       </c>
@@ -18142,9 +18132,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B2" s="68" t="s">
         <v>441</v>
@@ -18192,9 +18182,9 @@
         <v>445</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B3" s="68" t="s">
         <v>441</v>
@@ -18242,9 +18232,9 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B4" s="68" t="s">
         <v>441</v>
@@ -18292,9 +18282,9 @@
         <v>449</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B5" s="68" t="s">
         <v>441</v>
@@ -18342,9 +18332,9 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B6" s="70" t="s">
         <v>441</v>
@@ -18392,9 +18382,9 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B7" s="70" t="s">
         <v>441</v>
@@ -18442,9 +18432,9 @@
         <v>454</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B8" s="68" t="s">
         <v>441</v>
@@ -18492,9 +18482,9 @@
         <v>456</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B9" s="68" t="s">
         <v>441</v>
@@ -18542,9 +18532,9 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>441</v>
@@ -18592,9 +18582,9 @@
         <v>458</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>441</v>
@@ -18642,9 +18632,9 @@
         <v>459</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>441</v>
@@ -18692,9 +18682,9 @@
         <v>460</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>441</v>
@@ -18742,9 +18732,9 @@
         <v>461</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>441</v>
@@ -18792,9 +18782,9 @@
         <v>462</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>441</v>
@@ -18842,9 +18832,9 @@
         <v>463</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>441</v>
@@ -18892,9 +18882,9 @@
         <v>464</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>441</v>
@@ -18942,9 +18932,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>441</v>
@@ -18992,9 +18982,9 @@
         <v>466</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="39">
       <c r="A19" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B19" s="68" t="s">
         <v>467</v>
@@ -19042,9 +19032,9 @@
         <v>470</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="39">
       <c r="A20" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B20" s="68" t="s">
         <v>467</v>
@@ -19092,9 +19082,9 @@
         <v>472</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="39">
       <c r="A21" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B21" s="68" t="s">
         <v>467</v>
@@ -19142,9 +19132,9 @@
         <v>473</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="39">
       <c r="A22" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B22" s="68" t="s">
         <v>467</v>
@@ -19192,9 +19182,9 @@
         <v>474</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="39">
       <c r="A23" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B23" s="68" t="s">
         <v>467</v>
@@ -19242,9 +19232,9 @@
         <v>475</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="39">
       <c r="A24" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B24" s="68" t="s">
         <v>467</v>
@@ -19292,9 +19282,9 @@
         <v>476</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="39">
       <c r="A25" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B25" s="68" t="s">
         <v>467</v>
@@ -19342,9 +19332,9 @@
         <v>477</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="26.25">
       <c r="A26" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B26" s="68" t="s">
         <v>467</v>
@@ -19392,9 +19382,9 @@
         <v>478</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="39">
       <c r="A27" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B27" s="68" t="s">
         <v>467</v>
@@ -19442,9 +19432,9 @@
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="39">
       <c r="A28" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B28" s="68" t="s">
         <v>467</v>
@@ -19492,9 +19482,9 @@
         <v>480</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="39">
       <c r="A29" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B29" s="68" t="s">
         <v>467</v>
@@ -19542,9 +19532,9 @@
         <v>481</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>482</v>
@@ -19592,9 +19582,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>482</v>
@@ -19642,9 +19632,9 @@
         <v>485</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16">
       <c r="A32" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>482</v>
@@ -19692,9 +19682,9 @@
         <v>486</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>482</v>
@@ -19742,9 +19732,9 @@
         <v>487</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>482</v>
@@ -19792,9 +19782,9 @@
         <v>488</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>482</v>
@@ -19842,9 +19832,9 @@
         <v>490</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>482</v>
@@ -19892,9 +19882,9 @@
         <v>491</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>482</v>
@@ -19942,9 +19932,9 @@
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>482</v>
@@ -19992,9 +19982,9 @@
         <v>493</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="39">
       <c r="A39" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B39" s="68" t="s">
         <v>494</v>
@@ -20042,9 +20032,9 @@
         <v>495</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="39">
       <c r="A40" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B40" s="68" t="s">
         <v>494</v>
@@ -20092,9 +20082,9 @@
         <v>496</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="39">
       <c r="A41" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B41" s="68" t="s">
         <v>494</v>
@@ -20142,9 +20132,9 @@
         <v>497</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="39">
       <c r="A42" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B42" s="68" t="s">
         <v>494</v>
@@ -20192,9 +20182,9 @@
         <v>499</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="39">
       <c r="A43" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B43" s="68" t="s">
         <v>494</v>
@@ -20242,9 +20232,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="39">
       <c r="A44" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B44" s="68" t="s">
         <v>494</v>
@@ -20292,9 +20282,9 @@
         <v>501</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="39">
       <c r="A45" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B45" s="68" t="s">
         <v>494</v>
@@ -20342,9 +20332,9 @@
         <v>502</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="39">
       <c r="A46" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B46" s="68" t="s">
         <v>494</v>
@@ -20392,9 +20382,9 @@
         <v>504</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="39">
       <c r="A47" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B47" s="68" t="s">
         <v>494</v>
@@ -20442,9 +20432,9 @@
         <v>505</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="26.25">
       <c r="A48" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B48" s="68" t="s">
         <v>494</v>
@@ -20492,9 +20482,9 @@
         <v>506</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="39">
       <c r="A49" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B49" s="68" t="s">
         <v>494</v>
@@ -20542,9 +20532,9 @@
         <v>507</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="39">
       <c r="A50" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B50" s="68" t="s">
         <v>494</v>
@@ -20592,9 +20582,9 @@
         <v>508</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="39">
       <c r="A51" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B51" s="68" t="s">
         <v>494</v>
@@ -20642,9 +20632,9 @@
         <v>509</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="39">
       <c r="A52" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>494</v>
@@ -20692,9 +20682,9 @@
         <v>511</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="39">
       <c r="A53" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>494</v>
@@ -20742,9 +20732,9 @@
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="39">
       <c r="A54" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>494</v>
@@ -20792,9 +20782,9 @@
         <v>515</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="39">
       <c r="A55" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>494</v>
@@ -20842,9 +20832,9 @@
         <v>516</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="39">
       <c r="A56" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>494</v>
@@ -20892,9 +20882,9 @@
         <v>517</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="39">
       <c r="A57" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>494</v>
@@ -20942,9 +20932,9 @@
         <v>518</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="39">
       <c r="A58" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>494</v>
@@ -20992,9 +20982,9 @@
         <v>519</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="39">
       <c r="A59" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>494</v>
@@ -21042,9 +21032,9 @@
         <v>520</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="26.25">
       <c r="A60" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>494</v>
@@ -21092,9 +21082,9 @@
         <v>521</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="39">
       <c r="A61" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>494</v>
@@ -21142,9 +21132,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="39">
       <c r="A62" s="62" t="s">
-        <v>525</v>
+        <v>42</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>494</v>
@@ -21192,7 +21182,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16">
       <c r="A63" s="62"/>
       <c r="B63" s="68"/>
       <c r="C63" s="68"/>
@@ -21210,7 +21200,7 @@
       <c r="O63" s="68"/>
       <c r="P63" s="64"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16">
       <c r="A64" s="62"/>
       <c r="B64" s="62"/>
       <c r="C64" s="62"/>

</xml_diff>

<commit_message>
Update on 21st for single script
</commit_message>
<xml_diff>
--- a/Excels/Data_QA_Tests.xlsx
+++ b/Excels/Data_QA_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="11760" tabRatio="661" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="11760" tabRatio="661"/>
   </bookViews>
   <sheets>
     <sheet name="MBA Standard Reports" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5598" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5598" uniqueCount="526">
   <si>
     <t>Site Instance</t>
   </si>
@@ -1594,6 +1594,9 @@
   </si>
   <si>
     <t xml:space="preserve">Post Graduation  </t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -2185,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2298,7 +2301,7 @@
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -2345,7 +2348,7 @@
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -2392,7 +2395,7 @@
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -2439,7 +2442,7 @@
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -2486,7 +2489,7 @@
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -2533,7 +2536,7 @@
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>9</v>
@@ -2580,7 +2583,7 @@
     </row>
     <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>9</v>
@@ -2627,7 +2630,7 @@
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>9</v>
@@ -2674,7 +2677,7 @@
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>9</v>
@@ -2721,7 +2724,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
@@ -2768,7 +2771,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -2815,7 +2818,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
@@ -2862,7 +2865,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
@@ -2909,7 +2912,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
@@ -2956,7 +2959,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
@@ -3003,7 +3006,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
@@ -3050,7 +3053,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
@@ -3097,7 +3100,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>9</v>
@@ -3144,7 +3147,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>9</v>
@@ -3191,7 +3194,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>9</v>
@@ -3238,7 +3241,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>9</v>
@@ -3285,7 +3288,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>9</v>
@@ -3332,7 +3335,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>9</v>
@@ -3379,7 +3382,7 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>9</v>
@@ -3426,7 +3429,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>9</v>
@@ -3473,7 +3476,7 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>9</v>
@@ -3520,7 +3523,7 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>9</v>
@@ -3567,7 +3570,7 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>9</v>
@@ -3614,7 +3617,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>9</v>
@@ -3661,7 +3664,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>9</v>
@@ -3708,7 +3711,7 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>9</v>
@@ -3755,7 +3758,7 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>9</v>
@@ -3802,7 +3805,7 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>9</v>
@@ -3849,7 +3852,7 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>9</v>
@@ -3896,7 +3899,7 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>9</v>
@@ -3943,7 +3946,7 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>9</v>
@@ -3990,7 +3993,7 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>9</v>
@@ -4037,7 +4040,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>9</v>
@@ -4084,7 +4087,7 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>9</v>
@@ -4131,7 +4134,7 @@
     </row>
     <row r="42" spans="1:15" ht="26.25">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>9</v>
@@ -4178,7 +4181,7 @@
     </row>
     <row r="43" spans="1:15" ht="26.25">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>9</v>
@@ -4225,7 +4228,7 @@
     </row>
     <row r="44" spans="1:15" ht="26.25">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>9</v>
@@ -4272,7 +4275,7 @@
     </row>
     <row r="45" spans="1:15" ht="26.25">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>9</v>
@@ -4319,7 +4322,7 @@
     </row>
     <row r="46" spans="1:15" ht="26.25">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>9</v>
@@ -4366,7 +4369,7 @@
     </row>
     <row r="47" spans="1:15" ht="26.25">
       <c r="A47" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>9</v>
@@ -4413,7 +4416,7 @@
     </row>
     <row r="48" spans="1:15" ht="26.25">
       <c r="A48" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>9</v>
@@ -4460,7 +4463,7 @@
     </row>
     <row r="49" spans="1:15" ht="26.25">
       <c r="A49" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>9</v>
@@ -4507,7 +4510,7 @@
     </row>
     <row r="50" spans="1:15" ht="26.25">
       <c r="A50" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>9</v>
@@ -4554,7 +4557,7 @@
     </row>
     <row r="51" spans="1:15" ht="26.25">
       <c r="A51" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>9</v>
@@ -4601,7 +4604,7 @@
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>9</v>
@@ -4648,7 +4651,7 @@
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>9</v>
@@ -4695,7 +4698,7 @@
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>9</v>
@@ -4742,7 +4745,7 @@
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>9</v>
@@ -4789,7 +4792,7 @@
     </row>
     <row r="56" spans="1:15">
       <c r="A56" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>9</v>
@@ -4836,7 +4839,7 @@
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>9</v>
@@ -4883,7 +4886,7 @@
     </row>
     <row r="58" spans="1:15">
       <c r="A58" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>9</v>
@@ -4930,7 +4933,7 @@
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>9</v>
@@ -4977,7 +4980,7 @@
     </row>
     <row r="60" spans="1:15">
       <c r="A60" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>9</v>
@@ -5024,7 +5027,7 @@
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B61" s="19" t="s">
         <v>9</v>
@@ -5071,7 +5074,7 @@
     </row>
     <row r="62" spans="1:15" ht="26.25">
       <c r="A62" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>9</v>
@@ -5118,7 +5121,7 @@
     </row>
     <row r="63" spans="1:15" ht="26.25">
       <c r="A63" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>9</v>
@@ -5165,7 +5168,7 @@
     </row>
     <row r="64" spans="1:15" ht="26.25">
       <c r="A64" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>9</v>
@@ -5212,7 +5215,7 @@
     </row>
     <row r="65" spans="1:15" ht="26.25">
       <c r="A65" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>9</v>
@@ -5259,7 +5262,7 @@
     </row>
     <row r="66" spans="1:15" ht="26.25">
       <c r="A66" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>9</v>
@@ -5306,7 +5309,7 @@
     </row>
     <row r="67" spans="1:15" ht="26.25">
       <c r="A67" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>9</v>
@@ -5353,7 +5356,7 @@
     </row>
     <row r="68" spans="1:15" ht="26.25">
       <c r="A68" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>9</v>
@@ -5400,7 +5403,7 @@
     </row>
     <row r="69" spans="1:15" ht="26.25">
       <c r="A69" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>9</v>
@@ -5447,7 +5450,7 @@
     </row>
     <row r="70" spans="1:15" ht="26.25">
       <c r="A70" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>9</v>
@@ -5494,7 +5497,7 @@
     </row>
     <row r="71" spans="1:15" ht="26.25">
       <c r="A71" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>9</v>
@@ -5541,7 +5544,7 @@
     </row>
     <row r="72" spans="1:15">
       <c r="A72" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>9</v>
@@ -5588,7 +5591,7 @@
     </row>
     <row r="73" spans="1:15">
       <c r="A73" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>9</v>
@@ -5635,7 +5638,7 @@
     </row>
     <row r="74" spans="1:15">
       <c r="A74" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
@@ -5682,7 +5685,7 @@
     </row>
     <row r="75" spans="1:15">
       <c r="A75" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
@@ -5729,7 +5732,7 @@
     </row>
     <row r="76" spans="1:15">
       <c r="A76" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>9</v>
@@ -5776,7 +5779,7 @@
     </row>
     <row r="77" spans="1:15">
       <c r="A77" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>9</v>
@@ -5823,7 +5826,7 @@
     </row>
     <row r="78" spans="1:15">
       <c r="A78" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>9</v>
@@ -5870,7 +5873,7 @@
     </row>
     <row r="79" spans="1:15">
       <c r="A79" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>9</v>
@@ -5917,7 +5920,7 @@
     </row>
     <row r="80" spans="1:15">
       <c r="A80" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>9</v>
@@ -5964,7 +5967,7 @@
     </row>
     <row r="81" spans="1:15">
       <c r="A81" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>9</v>
@@ -6011,7 +6014,7 @@
     </row>
     <row r="82" spans="1:15">
       <c r="A82" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>9</v>
@@ -6058,7 +6061,7 @@
     </row>
     <row r="83" spans="1:15">
       <c r="A83" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>9</v>
@@ -6105,7 +6108,7 @@
     </row>
     <row r="84" spans="1:15">
       <c r="A84" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>9</v>
@@ -6152,7 +6155,7 @@
     </row>
     <row r="85" spans="1:15">
       <c r="A85" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>9</v>
@@ -6199,7 +6202,7 @@
     </row>
     <row r="86" spans="1:15">
       <c r="A86" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>9</v>
@@ -6246,7 +6249,7 @@
     </row>
     <row r="87" spans="1:15">
       <c r="A87" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>9</v>
@@ -6293,7 +6296,7 @@
     </row>
     <row r="88" spans="1:15">
       <c r="A88" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>9</v>
@@ -6340,7 +6343,7 @@
     </row>
     <row r="89" spans="1:15">
       <c r="A89" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>9</v>
@@ -6387,7 +6390,7 @@
     </row>
     <row r="90" spans="1:15">
       <c r="A90" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>9</v>
@@ -6434,7 +6437,7 @@
     </row>
     <row r="91" spans="1:15">
       <c r="A91" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>9</v>
@@ -6481,7 +6484,7 @@
     </row>
     <row r="92" spans="1:15" ht="26.25">
       <c r="A92" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>9</v>
@@ -6528,7 +6531,7 @@
     </row>
     <row r="93" spans="1:15" ht="26.25">
       <c r="A93" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>9</v>
@@ -6575,7 +6578,7 @@
     </row>
     <row r="94" spans="1:15" ht="26.25">
       <c r="A94" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>9</v>
@@ -6622,7 +6625,7 @@
     </row>
     <row r="95" spans="1:15" ht="26.25">
       <c r="A95" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>9</v>
@@ -6669,7 +6672,7 @@
     </row>
     <row r="96" spans="1:15" ht="26.25">
       <c r="A96" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>9</v>
@@ -6716,7 +6719,7 @@
     </row>
     <row r="97" spans="1:15" ht="26.25">
       <c r="A97" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>9</v>
@@ -6763,7 +6766,7 @@
     </row>
     <row r="98" spans="1:15" ht="26.25">
       <c r="A98" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>9</v>
@@ -6810,7 +6813,7 @@
     </row>
     <row r="99" spans="1:15" ht="26.25">
       <c r="A99" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>9</v>
@@ -6857,7 +6860,7 @@
     </row>
     <row r="100" spans="1:15" ht="26.25">
       <c r="A100" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>9</v>
@@ -6904,7 +6907,7 @@
     </row>
     <row r="101" spans="1:15" ht="26.25">
       <c r="A101" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B101" s="19" t="s">
         <v>9</v>
@@ -6951,7 +6954,7 @@
     </row>
     <row r="102" spans="1:15" ht="26.25">
       <c r="A102" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>9</v>
@@ -6998,7 +7001,7 @@
     </row>
     <row r="103" spans="1:15" ht="26.25">
       <c r="A103" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>9</v>
@@ -7045,7 +7048,7 @@
     </row>
     <row r="104" spans="1:15" ht="26.25">
       <c r="A104" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>9</v>
@@ -7092,7 +7095,7 @@
     </row>
     <row r="105" spans="1:15" ht="26.25">
       <c r="A105" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>9</v>
@@ -7139,7 +7142,7 @@
     </row>
     <row r="106" spans="1:15" ht="26.25">
       <c r="A106" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>9</v>
@@ -7186,7 +7189,7 @@
     </row>
     <row r="107" spans="1:15" ht="26.25">
       <c r="A107" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>9</v>
@@ -7233,7 +7236,7 @@
     </row>
     <row r="108" spans="1:15" ht="26.25">
       <c r="A108" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>9</v>
@@ -7280,7 +7283,7 @@
     </row>
     <row r="109" spans="1:15" ht="26.25">
       <c r="A109" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>9</v>
@@ -7327,7 +7330,7 @@
     </row>
     <row r="110" spans="1:15" ht="26.25">
       <c r="A110" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>9</v>
@@ -7374,7 +7377,7 @@
     </row>
     <row r="111" spans="1:15" ht="26.25">
       <c r="A111" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B111" s="19" t="s">
         <v>9</v>
@@ -7421,7 +7424,7 @@
     </row>
     <row r="112" spans="1:15" ht="26.25">
       <c r="A112" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>9</v>
@@ -7468,7 +7471,7 @@
     </row>
     <row r="113" spans="1:15" ht="26.25">
       <c r="A113" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>9</v>
@@ -7515,7 +7518,7 @@
     </row>
     <row r="114" spans="1:15" ht="26.25">
       <c r="A114" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>9</v>
@@ -7562,7 +7565,7 @@
     </row>
     <row r="115" spans="1:15" ht="26.25">
       <c r="A115" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>9</v>
@@ -7609,7 +7612,7 @@
     </row>
     <row r="116" spans="1:15" ht="26.25">
       <c r="A116" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>9</v>
@@ -7656,7 +7659,7 @@
     </row>
     <row r="117" spans="1:15" ht="26.25">
       <c r="A117" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>9</v>
@@ -7703,7 +7706,7 @@
     </row>
     <row r="118" spans="1:15" ht="26.25">
       <c r="A118" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>9</v>
@@ -7750,7 +7753,7 @@
     </row>
     <row r="119" spans="1:15" ht="26.25">
       <c r="A119" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>9</v>
@@ -7797,7 +7800,7 @@
     </row>
     <row r="120" spans="1:15" ht="26.25">
       <c r="A120" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>9</v>
@@ -7844,7 +7847,7 @@
     </row>
     <row r="121" spans="1:15" ht="26.25">
       <c r="A121" s="1" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B121" s="19" t="s">
         <v>9</v>
@@ -18059,8 +18062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18184,7 +18187,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B3" s="68" t="s">
         <v>441</v>
@@ -18234,7 +18237,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B4" s="68" t="s">
         <v>441</v>
@@ -18284,7 +18287,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B5" s="68" t="s">
         <v>441</v>
@@ -18334,7 +18337,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B6" s="70" t="s">
         <v>441</v>
@@ -18384,7 +18387,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B7" s="70" t="s">
         <v>441</v>
@@ -18434,7 +18437,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B8" s="68" t="s">
         <v>441</v>
@@ -18484,7 +18487,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B9" s="68" t="s">
         <v>441</v>
@@ -18534,7 +18537,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>441</v>
@@ -18584,7 +18587,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>441</v>
@@ -18634,7 +18637,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>441</v>
@@ -18684,7 +18687,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>441</v>
@@ -18734,7 +18737,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>441</v>
@@ -18784,7 +18787,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>441</v>
@@ -18834,7 +18837,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>441</v>
@@ -18884,7 +18887,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>441</v>
@@ -18934,7 +18937,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>441</v>
@@ -18984,7 +18987,7 @@
     </row>
     <row r="19" spans="1:16" ht="39">
       <c r="A19" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B19" s="68" t="s">
         <v>467</v>
@@ -19034,7 +19037,7 @@
     </row>
     <row r="20" spans="1:16" ht="39">
       <c r="A20" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B20" s="68" t="s">
         <v>467</v>
@@ -19084,7 +19087,7 @@
     </row>
     <row r="21" spans="1:16" ht="39">
       <c r="A21" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B21" s="68" t="s">
         <v>467</v>
@@ -19134,7 +19137,7 @@
     </row>
     <row r="22" spans="1:16" ht="39">
       <c r="A22" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B22" s="68" t="s">
         <v>467</v>
@@ -19184,7 +19187,7 @@
     </row>
     <row r="23" spans="1:16" ht="39">
       <c r="A23" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B23" s="68" t="s">
         <v>467</v>
@@ -19234,7 +19237,7 @@
     </row>
     <row r="24" spans="1:16" ht="39">
       <c r="A24" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B24" s="68" t="s">
         <v>467</v>
@@ -19284,7 +19287,7 @@
     </row>
     <row r="25" spans="1:16" ht="39">
       <c r="A25" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B25" s="68" t="s">
         <v>467</v>
@@ -19334,7 +19337,7 @@
     </row>
     <row r="26" spans="1:16" ht="26.25">
       <c r="A26" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B26" s="68" t="s">
         <v>467</v>
@@ -19384,7 +19387,7 @@
     </row>
     <row r="27" spans="1:16" ht="39">
       <c r="A27" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B27" s="68" t="s">
         <v>467</v>
@@ -19434,7 +19437,7 @@
     </row>
     <row r="28" spans="1:16" ht="39">
       <c r="A28" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B28" s="68" t="s">
         <v>467</v>
@@ -19484,7 +19487,7 @@
     </row>
     <row r="29" spans="1:16" ht="39">
       <c r="A29" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B29" s="68" t="s">
         <v>467</v>
@@ -19534,7 +19537,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>482</v>
@@ -19584,7 +19587,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>482</v>
@@ -19634,7 +19637,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>482</v>
@@ -19684,7 +19687,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>482</v>
@@ -19734,7 +19737,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>482</v>
@@ -19784,7 +19787,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>482</v>
@@ -19834,7 +19837,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>482</v>
@@ -19884,7 +19887,7 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>482</v>
@@ -19934,7 +19937,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>482</v>
@@ -19984,7 +19987,7 @@
     </row>
     <row r="39" spans="1:16" ht="39">
       <c r="A39" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B39" s="68" t="s">
         <v>494</v>
@@ -20034,7 +20037,7 @@
     </row>
     <row r="40" spans="1:16" ht="39">
       <c r="A40" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B40" s="68" t="s">
         <v>494</v>
@@ -20084,7 +20087,7 @@
     </row>
     <row r="41" spans="1:16" ht="39">
       <c r="A41" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B41" s="68" t="s">
         <v>494</v>
@@ -20134,7 +20137,7 @@
     </row>
     <row r="42" spans="1:16" ht="39">
       <c r="A42" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B42" s="68" t="s">
         <v>494</v>
@@ -20184,7 +20187,7 @@
     </row>
     <row r="43" spans="1:16" ht="39">
       <c r="A43" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B43" s="68" t="s">
         <v>494</v>
@@ -20234,7 +20237,7 @@
     </row>
     <row r="44" spans="1:16" ht="39">
       <c r="A44" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B44" s="68" t="s">
         <v>494</v>
@@ -20284,7 +20287,7 @@
     </row>
     <row r="45" spans="1:16" ht="39">
       <c r="A45" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B45" s="68" t="s">
         <v>494</v>
@@ -20334,7 +20337,7 @@
     </row>
     <row r="46" spans="1:16" ht="39">
       <c r="A46" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B46" s="68" t="s">
         <v>494</v>
@@ -20384,7 +20387,7 @@
     </row>
     <row r="47" spans="1:16" ht="39">
       <c r="A47" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B47" s="68" t="s">
         <v>494</v>
@@ -20434,7 +20437,7 @@
     </row>
     <row r="48" spans="1:16" ht="26.25">
       <c r="A48" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B48" s="68" t="s">
         <v>494</v>
@@ -20484,7 +20487,7 @@
     </row>
     <row r="49" spans="1:16" ht="39">
       <c r="A49" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B49" s="68" t="s">
         <v>494</v>
@@ -20534,7 +20537,7 @@
     </row>
     <row r="50" spans="1:16" ht="39">
       <c r="A50" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B50" s="68" t="s">
         <v>494</v>
@@ -20584,7 +20587,7 @@
     </row>
     <row r="51" spans="1:16" ht="39">
       <c r="A51" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B51" s="68" t="s">
         <v>494</v>
@@ -20634,7 +20637,7 @@
     </row>
     <row r="52" spans="1:16" ht="39">
       <c r="A52" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>494</v>
@@ -20684,7 +20687,7 @@
     </row>
     <row r="53" spans="1:16" ht="39">
       <c r="A53" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>494</v>
@@ -20734,7 +20737,7 @@
     </row>
     <row r="54" spans="1:16" ht="39">
       <c r="A54" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>494</v>
@@ -20784,7 +20787,7 @@
     </row>
     <row r="55" spans="1:16" ht="39">
       <c r="A55" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>494</v>
@@ -20834,7 +20837,7 @@
     </row>
     <row r="56" spans="1:16" ht="39">
       <c r="A56" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>494</v>
@@ -20884,7 +20887,7 @@
     </row>
     <row r="57" spans="1:16" ht="39">
       <c r="A57" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>494</v>
@@ -20934,7 +20937,7 @@
     </row>
     <row r="58" spans="1:16" ht="39">
       <c r="A58" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>494</v>
@@ -20984,7 +20987,7 @@
     </row>
     <row r="59" spans="1:16" ht="39">
       <c r="A59" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>494</v>
@@ -21034,7 +21037,7 @@
     </row>
     <row r="60" spans="1:16" ht="26.25">
       <c r="A60" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>494</v>
@@ -21084,7 +21087,7 @@
     </row>
     <row r="61" spans="1:16" ht="39">
       <c r="A61" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>494</v>
@@ -21134,7 +21137,7 @@
     </row>
     <row r="62" spans="1:16" ht="39">
       <c r="A62" s="62" t="s">
-        <v>42</v>
+        <v>525</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>494</v>

</xml_diff>